<commit_message>
refactored payment test cases
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Order/order_payment_test_data.xlsx
+++ b/TestData/Web_POS/Order/order_payment_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110" count="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112" count="839">
   <si>
     <t>TC_Id</t>
   </si>
@@ -345,6 +345,12 @@
   <si>
     <t>O_P_87</t>
   </si>
+  <si>
+    <t>307260624cAE</t>
+  </si>
+  <si>
+    <t>userone_p13</t>
+  </si>
 </sst>
 </file>
 
@@ -406,7 +412,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none">
         <fgColor indexed="64"/>
@@ -431,6 +437,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -452,7 +464,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1">
@@ -467,6 +479,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,6 +698,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" customHeight="true" defaultRowHeight="15.75"/>
   <cols>
+    <col min="5" max="5" width="41.59765625" customWidth="1"/>
     <col min="10" max="12" width="28.9296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -989,7 +1003,7 @@
         <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
@@ -997,8 +1011,8 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
+      <c r="E5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>27</v>
@@ -1062,7 +1076,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
@@ -1071,7 +1085,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -1135,7 +1149,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -1143,8 +1157,8 @@
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
+      <c r="E7" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>27</v>
@@ -1208,7 +1222,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -1217,7 +1231,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>27</v>

</xml_diff>